<commit_message>
Cambio cuentas por pagar pagos pendientes
</commit_message>
<xml_diff>
--- a/Ppgz/Ppgz.Web/App_Data/plantillapagospendientes.xlsx
+++ b/Ppgz/Ppgz.Web/App_Data/plantillapagospendientes.xlsx
@@ -36,9 +36,6 @@
     <t>ML</t>
   </si>
   <si>
-    <t>FECHA</t>
-  </si>
-  <si>
     <t>TIPO MOVIMIENTO</t>
   </si>
   <si>
@@ -51,10 +48,13 @@
     <t>Total:</t>
   </si>
   <si>
-    <t>FECHA DOC.</t>
+    <t>VENCIMIENTO</t>
   </si>
   <si>
-    <t>TEXTO</t>
+    <t>FECHA DE DOCUMENTO</t>
+  </si>
+  <si>
+    <t>DESCRIPCIÓN</t>
   </si>
 </sst>
 </file>
@@ -678,15 +678,15 @@
     <col min="1" max="1" width="14" style="11" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" style="12" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.42578125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -726,7 +726,7 @@
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="5"/>
@@ -735,7 +735,7 @@
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="5"/>
@@ -760,10 +760,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>10</v>

</xml_diff>